<commit_message>
Trabajo terminado v2. Revisar para entrega.
</commit_message>
<xml_diff>
--- a/TP N1/VALORES_100Ciclos__Torneo__Elitismo.xlsx
+++ b/TP N1/VALORES_100Ciclos__Torneo__Elitismo.xlsx
@@ -435,7 +435,7 @@
   <cols>
     <col width="9" customWidth="1" min="1" max="1"/>
     <col width="20" customWidth="1" min="2" max="2"/>
-    <col width="22" customWidth="1" min="3" max="3"/>
+    <col width="21" customWidth="1" min="3" max="3"/>
     <col width="8" customWidth="1" min="4" max="4"/>
     <col width="12" customWidth="1" min="5" max="5"/>
     <col width="32" customWidth="1" min="6" max="6"/>
@@ -478,22 +478,22 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>0.9313985248163243</v>
+        <v>0.8644407273223967</v>
       </c>
       <c r="C2" t="n">
-        <v>0.07310323318009376</v>
+        <v>0.2061176298559729</v>
       </c>
       <c r="D2" t="n">
-        <v>0.5472</v>
+        <v>0.5149</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>1036257394</t>
+          <t>998314731</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>111101110001000000100001110010</t>
+          <t>111011100000010001001011101011</t>
         </is>
       </c>
     </row>
@@ -502,22 +502,22 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>0.9313985248163243</v>
+        <v>0.8644407273223967</v>
       </c>
       <c r="C3" t="n">
-        <v>0.7733646957901678</v>
+        <v>0.3066808315735384</v>
       </c>
       <c r="D3" t="n">
-        <v>0.7915</v>
+        <v>0.6511</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>1036257394</t>
+          <t>998314731</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>111101110001000000100001110010</t>
+          <t>111011100000010001001011101011</t>
         </is>
       </c>
     </row>
@@ -526,22 +526,22 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>0.9313985248163243</v>
+        <v>0.8644407273223967</v>
       </c>
       <c r="C4" t="n">
-        <v>0.7733647416550555</v>
+        <v>0.6451797487666932</v>
       </c>
       <c r="D4" t="n">
-        <v>0.7915</v>
+        <v>0.7246</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>1036257394</t>
+          <t>998314731</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>111101110001000000100001110010</t>
+          <t>111011100000010001001011101011</t>
         </is>
       </c>
     </row>
@@ -550,22 +550,22 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>0.9313985248163243</v>
+        <v>0.8644407273223967</v>
       </c>
       <c r="C5" t="n">
-        <v>0.7733647416550555</v>
+        <v>0.6666041260667456</v>
       </c>
       <c r="D5" t="n">
-        <v>0.7915</v>
+        <v>0.723</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>1036257394</t>
+          <t>998314731</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>111101110001000000100001110010</t>
+          <t>111011100000010001001011101011</t>
         </is>
       </c>
     </row>
@@ -574,22 +574,22 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>0.9313985248163243</v>
+        <v>0.8644407273223967</v>
       </c>
       <c r="C6" t="n">
-        <v>0.7733646957901678</v>
+        <v>0.7037118534958166</v>
       </c>
       <c r="D6" t="n">
-        <v>0.7915</v>
+        <v>0.7305</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>1036257394</t>
+          <t>998314731</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>111101110001000000100001110010</t>
+          <t>111011100000010001001011101011</t>
         </is>
       </c>
     </row>
@@ -598,22 +598,22 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>0.9313985248163243</v>
+        <v>0.8644407273223967</v>
       </c>
       <c r="C7" t="n">
-        <v>0.7733646957901678</v>
+        <v>0.7037118503707623</v>
       </c>
       <c r="D7" t="n">
-        <v>0.7915</v>
+        <v>0.7305</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>1036257394</t>
+          <t>998314731</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>111101110001000000100001110010</t>
+          <t>111011100000010001001011101011</t>
         </is>
       </c>
     </row>
@@ -622,22 +622,22 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>0.9313985248163243</v>
+        <v>0.8644407273223967</v>
       </c>
       <c r="C8" t="n">
-        <v>0.7733646957901678</v>
+        <v>0.7037118534958166</v>
       </c>
       <c r="D8" t="n">
-        <v>0.7915</v>
+        <v>0.7305</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>1036257394</t>
+          <t>998314731</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>111101110001000000100001110010</t>
+          <t>111011100000010001001011101011</t>
         </is>
       </c>
     </row>
@@ -646,22 +646,22 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>0.9313985248163243</v>
+        <v>0.8644407273223967</v>
       </c>
       <c r="C9" t="n">
-        <v>0.7733646957901678</v>
+        <v>0.7037118534958166</v>
       </c>
       <c r="D9" t="n">
-        <v>0.7915</v>
+        <v>0.7442</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>1036257394</t>
+          <t>998314731</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>111101110001000000100001110010</t>
+          <t>111011100000010001001011101011</t>
         </is>
       </c>
     </row>
@@ -670,22 +670,22 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>0.9313985248163243</v>
+        <v>0.8644407273223967</v>
       </c>
       <c r="C10" t="n">
-        <v>0.7733646957901678</v>
+        <v>0.7037118534958166</v>
       </c>
       <c r="D10" t="n">
-        <v>0.7915</v>
+        <v>0.7655999999999999</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>1036257394</t>
+          <t>998314731</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>111101110001000000100001110010</t>
+          <t>111011100000010001001011101011</t>
         </is>
       </c>
     </row>
@@ -694,22 +694,22 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>0.9313985248163243</v>
+        <v>0.8644407273223967</v>
       </c>
       <c r="C11" t="n">
-        <v>0.7733646957901678</v>
+        <v>0.7044032352191537</v>
       </c>
       <c r="D11" t="n">
-        <v>0.7915</v>
+        <v>0.7871</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>1036257394</t>
+          <t>998314731</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>111101110001000000100001110010</t>
+          <t>111011100000010001001011101011</t>
         </is>
       </c>
     </row>
@@ -718,22 +718,22 @@
         <v>11</v>
       </c>
       <c r="B12" t="n">
-        <v>0.9313985248163243</v>
+        <v>0.8644407273223967</v>
       </c>
       <c r="C12" t="n">
-        <v>0.773363483647198</v>
+        <v>0.8105805948869638</v>
       </c>
       <c r="D12" t="n">
-        <v>0.7915</v>
+        <v>0.819</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>1036257394</t>
+          <t>998314731</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>111101110001000000100001110010</t>
+          <t>111011100000010001001011101011</t>
         </is>
       </c>
     </row>
@@ -742,22 +742,22 @@
         <v>12</v>
       </c>
       <c r="B13" t="n">
-        <v>0.9313985248163243</v>
+        <v>0.8644407273223967</v>
       </c>
       <c r="C13" t="n">
-        <v>0.7733634901993196</v>
+        <v>0.8105329408089404</v>
       </c>
       <c r="D13" t="n">
-        <v>0.7915</v>
+        <v>0.819</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>1036257394</t>
+          <t>998314731</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>111101110001000000100001110010</t>
+          <t>111011100000010001001011101011</t>
         </is>
       </c>
     </row>
@@ -766,22 +766,22 @@
         <v>13</v>
       </c>
       <c r="B14" t="n">
-        <v>0.9313985248163243</v>
+        <v>0.8644407273223967</v>
       </c>
       <c r="C14" t="n">
-        <v>0.7733634377823475</v>
+        <v>0.8105805948869638</v>
       </c>
       <c r="D14" t="n">
-        <v>0.7915</v>
+        <v>0.819</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>1036257394</t>
+          <t>998314731</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>111101110001000000100001110010</t>
+          <t>111011100000010001001011101011</t>
         </is>
       </c>
     </row>
@@ -790,22 +790,22 @@
         <v>14</v>
       </c>
       <c r="B15" t="n">
-        <v>0.9313985248163243</v>
+        <v>0.8644407273223967</v>
       </c>
       <c r="C15" t="n">
-        <v>0.7733635426162934</v>
+        <v>0.8105805948869638</v>
       </c>
       <c r="D15" t="n">
-        <v>0.7916</v>
+        <v>0.819</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>1036257394</t>
+          <t>998314731</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>111101110001000000100001110010</t>
+          <t>111011100000010001001011101011</t>
         </is>
       </c>
     </row>
@@ -814,22 +814,22 @@
         <v>15</v>
       </c>
       <c r="B16" t="n">
-        <v>0.9313985248163243</v>
+        <v>0.8644407273223967</v>
       </c>
       <c r="C16" t="n">
-        <v>0.7733651675433642</v>
+        <v>0.8105800565760465</v>
       </c>
       <c r="D16" t="n">
-        <v>0.7917999999999999</v>
+        <v>0.819</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>1036257394</t>
+          <t>998314731</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>111101110001000000100001110010</t>
+          <t>111011100000010001001011101011</t>
         </is>
       </c>
     </row>
@@ -838,22 +838,22 @@
         <v>16</v>
       </c>
       <c r="B17" t="n">
-        <v>0.9313985248163243</v>
+        <v>0.8644407273223967</v>
       </c>
       <c r="C17" t="n">
-        <v>0.7733680504826907</v>
+        <v>0.8105800565760465</v>
       </c>
       <c r="D17" t="n">
-        <v>0.7921</v>
+        <v>0.819</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>1036257394</t>
+          <t>998314731</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>111101110001000000100001110010</t>
+          <t>111011100000010001001011101011</t>
         </is>
       </c>
     </row>
@@ -862,22 +862,22 @@
         <v>17</v>
       </c>
       <c r="B18" t="n">
-        <v>0.9313985248163243</v>
+        <v>0.8644407273223967</v>
       </c>
       <c r="C18" t="n">
-        <v>0.7743031400213035</v>
+        <v>0.8105800565760465</v>
       </c>
       <c r="D18" t="n">
-        <v>0.7922</v>
+        <v>0.819</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>1036257394</t>
+          <t>998314731</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>111101110001000000100001110010</t>
+          <t>111011100000010001001011101011</t>
         </is>
       </c>
     </row>
@@ -886,22 +886,22 @@
         <v>18</v>
       </c>
       <c r="B19" t="n">
-        <v>0.9313985248163243</v>
+        <v>0.8644407273223967</v>
       </c>
       <c r="C19" t="n">
-        <v>0.7743030875724973</v>
+        <v>0.8105800565760465</v>
       </c>
       <c r="D19" t="n">
-        <v>0.7922</v>
+        <v>0.819</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>1036257394</t>
+          <t>998314731</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>111101110001000000100001110010</t>
+          <t>111011100000010001001011101011</t>
         </is>
       </c>
     </row>
@@ -910,22 +910,22 @@
         <v>19</v>
       </c>
       <c r="B20" t="n">
-        <v>0.9313985248163243</v>
+        <v>0.8644407273223967</v>
       </c>
       <c r="C20" t="n">
-        <v>0.004427302045808749</v>
+        <v>0.8105797362727505</v>
       </c>
       <c r="D20" t="n">
-        <v>0.6383</v>
+        <v>0.819</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>1036257394</t>
+          <t>998314731</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>111101110001000000100001110010</t>
+          <t>111011100000010001001011101011</t>
         </is>
       </c>
     </row>
@@ -934,22 +934,22 @@
         <v>20</v>
       </c>
       <c r="B21" t="n">
-        <v>0.9313985248163243</v>
+        <v>0.8644407273223967</v>
       </c>
       <c r="C21" t="n">
-        <v>0.7743030875724973</v>
+        <v>0.8105797362727505</v>
       </c>
       <c r="D21" t="n">
-        <v>0.7922</v>
+        <v>0.819</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>1036257394</t>
+          <t>998314731</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>111101110001000000100001110010</t>
+          <t>111011100000010001001011101011</t>
         </is>
       </c>
     </row>
@@ -958,22 +958,22 @@
         <v>21</v>
       </c>
       <c r="B22" t="n">
-        <v>0.9313985248163243</v>
+        <v>0.8644407273223967</v>
       </c>
       <c r="C22" t="n">
-        <v>0.7743030875724973</v>
+        <v>0.8105797362727505</v>
       </c>
       <c r="D22" t="n">
-        <v>0.7922</v>
+        <v>0.819</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>1036257394</t>
+          <t>998314731</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>111101110001000000100001110010</t>
+          <t>111011100000010001001011101011</t>
         </is>
       </c>
     </row>
@@ -982,22 +982,22 @@
         <v>22</v>
       </c>
       <c r="B23" t="n">
-        <v>0.9313985248163243</v>
+        <v>0.8644407273223967</v>
       </c>
       <c r="C23" t="n">
-        <v>0.7743030875724973</v>
+        <v>0.8105805948869638</v>
       </c>
       <c r="D23" t="n">
-        <v>0.7922</v>
+        <v>0.819</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>1036257394</t>
+          <t>998314731</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>111101110001000000100001110010</t>
+          <t>111011100000010001001011101011</t>
         </is>
       </c>
     </row>
@@ -1006,22 +1006,22 @@
         <v>23</v>
       </c>
       <c r="B24" t="n">
-        <v>0.9313985248163243</v>
+        <v>0.8644407273223967</v>
       </c>
       <c r="C24" t="n">
-        <v>0.7743030875724973</v>
+        <v>0.8105805948869638</v>
       </c>
       <c r="D24" t="n">
-        <v>0.7922</v>
+        <v>0.819</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>1036257394</t>
+          <t>998314731</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>111101110001000000100001110010</t>
+          <t>111011100000010001001011101011</t>
         </is>
       </c>
     </row>
@@ -1030,22 +1030,22 @@
         <v>24</v>
       </c>
       <c r="B25" t="n">
-        <v>0.9313985248163243</v>
+        <v>0.8644407273223967</v>
       </c>
       <c r="C25" t="n">
-        <v>0.7743030875724973</v>
+        <v>0.8105805948869638</v>
       </c>
       <c r="D25" t="n">
-        <v>0.7922</v>
+        <v>0.819</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>1036257394</t>
+          <t>998314731</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>111101110001000000100001110010</t>
+          <t>111011100000010001001011101011</t>
         </is>
       </c>
     </row>
@@ -1054,22 +1054,22 @@
         <v>25</v>
       </c>
       <c r="B26" t="n">
-        <v>0.9313985248163243</v>
+        <v>0.8644407273223967</v>
       </c>
       <c r="C26" t="n">
-        <v>0.7743030875724973</v>
+        <v>0.8105805948869638</v>
       </c>
       <c r="D26" t="n">
-        <v>0.7922</v>
+        <v>0.819</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>1036257394</t>
+          <t>998314731</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>111101110001000000100001110010</t>
+          <t>111011100000010001001011101011</t>
         </is>
       </c>
     </row>
@@ -1078,22 +1078,22 @@
         <v>26</v>
       </c>
       <c r="B27" t="n">
-        <v>0.9313985248163243</v>
+        <v>0.8644407273223967</v>
       </c>
       <c r="C27" t="n">
-        <v>0.7743030875724973</v>
+        <v>0.8105805948869638</v>
       </c>
       <c r="D27" t="n">
-        <v>0.7922</v>
+        <v>0.819</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>1036257394</t>
+          <t>998314731</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>111101110001000000100001110010</t>
+          <t>111011100000010001001011101011</t>
         </is>
       </c>
     </row>
@@ -1102,22 +1102,22 @@
         <v>27</v>
       </c>
       <c r="B28" t="n">
-        <v>0.9313985248163243</v>
+        <v>0.8644407273223967</v>
       </c>
       <c r="C28" t="n">
-        <v>0.7743030875724973</v>
+        <v>0.8105805948869638</v>
       </c>
       <c r="D28" t="n">
-        <v>0.7922</v>
+        <v>0.819</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>1036257394</t>
+          <t>998314731</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>111101110001000000100001110010</t>
+          <t>111011100000010001001011101011</t>
         </is>
       </c>
     </row>
@@ -1126,22 +1126,22 @@
         <v>28</v>
       </c>
       <c r="B29" t="n">
-        <v>0.9313985248163243</v>
+        <v>0.8644407273223967</v>
       </c>
       <c r="C29" t="n">
-        <v>0.7743030875724973</v>
+        <v>0.8105805948869638</v>
       </c>
       <c r="D29" t="n">
-        <v>0.7922</v>
+        <v>0.819</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>1036257394</t>
+          <t>998314731</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>111101110001000000100001110010</t>
+          <t>111011100000010001001011101011</t>
         </is>
       </c>
     </row>
@@ -1150,22 +1150,22 @@
         <v>29</v>
       </c>
       <c r="B30" t="n">
-        <v>0.9313985248163243</v>
+        <v>0.8644407273223967</v>
       </c>
       <c r="C30" t="n">
-        <v>0.7743030875724973</v>
+        <v>0.8105805948869638</v>
       </c>
       <c r="D30" t="n">
-        <v>0.7922</v>
+        <v>0.819</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>1036257394</t>
+          <t>998314731</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>111101110001000000100001110010</t>
+          <t>111011100000010001001011101011</t>
         </is>
       </c>
     </row>
@@ -1174,22 +1174,22 @@
         <v>30</v>
       </c>
       <c r="B31" t="n">
-        <v>0.9313985248163243</v>
+        <v>0.8644407273223967</v>
       </c>
       <c r="C31" t="n">
-        <v>0.7743030875724973</v>
+        <v>0.8105805948869638</v>
       </c>
       <c r="D31" t="n">
-        <v>0.7922</v>
+        <v>0.819</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>1036257394</t>
+          <t>998314731</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>111101110001000000100001110010</t>
+          <t>111011100000010001001011101011</t>
         </is>
       </c>
     </row>
@@ -1198,22 +1198,22 @@
         <v>31</v>
       </c>
       <c r="B32" t="n">
-        <v>0.9313985248163243</v>
+        <v>0.8644407273223967</v>
       </c>
       <c r="C32" t="n">
-        <v>0.7743030875724973</v>
+        <v>0.8105805948869638</v>
       </c>
       <c r="D32" t="n">
-        <v>0.7922</v>
+        <v>0.819</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>1036257394</t>
+          <t>998314731</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>111101110001000000100001110010</t>
+          <t>111011100000010001001011101011</t>
         </is>
       </c>
     </row>
@@ -1222,22 +1222,22 @@
         <v>32</v>
       </c>
       <c r="B33" t="n">
-        <v>0.9313985248163243</v>
+        <v>0.8971830944948723</v>
       </c>
       <c r="C33" t="n">
-        <v>0.7743047659351761</v>
+        <v>0.8105805948869638</v>
       </c>
       <c r="D33" t="n">
-        <v>0.7922</v>
+        <v>0.8363</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>1036257394</t>
+          <t>1017045565</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>111101110001000000100001110010</t>
+          <t>111100100111101110001000111101</t>
         </is>
       </c>
     </row>
@@ -1246,22 +1246,22 @@
         <v>33</v>
       </c>
       <c r="B34" t="n">
-        <v>0.9313985248163243</v>
+        <v>0.9538023411342968</v>
       </c>
       <c r="C34" t="n">
-        <v>0.7743047659351761</v>
+        <v>0.8105805948869638</v>
       </c>
       <c r="D34" t="n">
-        <v>0.7922</v>
+        <v>0.8692</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>1036257394</t>
+          <t>1048646379</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>111101110001000000100001110010</t>
+          <t>111110100000010001001011101011</t>
         </is>
       </c>
     </row>
@@ -1270,22 +1270,22 @@
         <v>34</v>
       </c>
       <c r="B35" t="n">
-        <v>0.9313985248163243</v>
+        <v>0.9538023411342968</v>
       </c>
       <c r="C35" t="n">
-        <v>0.774304764296149</v>
+        <v>0.8644407273223967</v>
       </c>
       <c r="D35" t="n">
-        <v>0.7922</v>
+        <v>0.9076</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>1036257394</t>
+          <t>1048646379</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>111101110001000000100001110010</t>
+          <t>111110100000010001001011101011</t>
         </is>
       </c>
     </row>
@@ -1294,22 +1294,22 @@
         <v>35</v>
       </c>
       <c r="B36" t="n">
-        <v>0.9313985248163243</v>
+        <v>0.9573595004880254</v>
       </c>
       <c r="C36" t="n">
-        <v>0.7743047659351761</v>
+        <v>0.8937396506754539</v>
       </c>
       <c r="D36" t="n">
-        <v>0.7922</v>
+        <v>0.9368</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>1036257394</t>
+          <t>1050599997</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>111101110001000000100001110010</t>
+          <t>111110100111101110001000111101</t>
         </is>
       </c>
     </row>
@@ -1318,22 +1318,22 @@
         <v>36</v>
       </c>
       <c r="B37" t="n">
-        <v>0.9313985248163243</v>
+        <v>0.9573822126237355</v>
       </c>
       <c r="C37" t="n">
-        <v>0.7743047659351761</v>
+        <v>0.9537796715015481</v>
       </c>
       <c r="D37" t="n">
-        <v>0.7922</v>
+        <v>0.9556</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>1036257394</t>
+          <t>1050612459</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>111101110001000000100001110010</t>
+          <t>111110100111110001001011101011</t>
         </is>
       </c>
     </row>
@@ -1342,22 +1342,22 @@
         <v>37</v>
       </c>
       <c r="B38" t="n">
-        <v>0.9313985248163243</v>
+        <v>0.9573598176031357</v>
       </c>
       <c r="C38" t="n">
-        <v>0.4326717908756434</v>
+        <v>0.9538020246089228</v>
       </c>
       <c r="D38" t="n">
-        <v>0.7581</v>
+        <v>0.9566</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>1036257394</t>
+          <t>1050600171</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>111101110001000000100001110010</t>
+          <t>111110100111101110001011101011</t>
         </is>
       </c>
     </row>
@@ -1366,22 +1366,22 @@
         <v>38</v>
       </c>
       <c r="B39" t="n">
-        <v>0.9313985248163243</v>
+        <v>0.9573598176031357</v>
       </c>
       <c r="C39" t="n">
-        <v>0.7743047659351761</v>
+        <v>0.9573595004880254</v>
       </c>
       <c r="D39" t="n">
-        <v>0.7922</v>
+        <v>0.9574</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>1036257394</t>
+          <t>1050600171</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>111101110001000000100001110010</t>
+          <t>111110100111101110001011101011</t>
         </is>
       </c>
     </row>
@@ -1390,22 +1390,22 @@
         <v>39</v>
       </c>
       <c r="B40" t="n">
-        <v>0.9313985248163243</v>
+        <v>0.9669685027656603</v>
       </c>
       <c r="C40" t="n">
-        <v>0.7742078434711834</v>
+        <v>0.9573595004880254</v>
       </c>
       <c r="D40" t="n">
-        <v>0.7922</v>
+        <v>0.9583</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>1036257394</t>
+          <t>1055859261</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>111101110001000000100001110010</t>
+          <t>111110111011110010001000111101</t>
         </is>
       </c>
     </row>
@@ -1414,22 +1414,22 @@
         <v>40</v>
       </c>
       <c r="B41" t="n">
-        <v>0.9313985248163243</v>
+        <v>0.9669688178049883</v>
       </c>
       <c r="C41" t="n">
-        <v>0.7729331543157072</v>
+        <v>0.9008872034944768</v>
       </c>
       <c r="D41" t="n">
-        <v>0.7921</v>
+        <v>0.9556</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>1036257394</t>
+          <t>1055859433</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>111101110001000000100001110010</t>
+          <t>111110111011110010001011101001</t>
         </is>
       </c>
     </row>
@@ -1438,22 +1438,22 @@
         <v>41</v>
       </c>
       <c r="B42" t="n">
-        <v>0.9313985248163243</v>
+        <v>0.9669688178049883</v>
       </c>
       <c r="C42" t="n">
-        <v>0.7743047659351761</v>
+        <v>0.9573595041330264</v>
       </c>
       <c r="D42" t="n">
-        <v>0.7922</v>
+        <v>0.966</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>1036257394</t>
+          <t>1055859433</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>111101110001000000100001110010</t>
+          <t>111110111011110010001011101001</t>
         </is>
       </c>
     </row>
@@ -1462,22 +1462,22 @@
         <v>42</v>
       </c>
       <c r="B43" t="n">
-        <v>0.9313985248163243</v>
+        <v>0.966968825131485</v>
       </c>
       <c r="C43" t="n">
-        <v>0.7743047659351761</v>
+        <v>0.9669684954391649</v>
       </c>
       <c r="D43" t="n">
-        <v>0.7922</v>
+        <v>0.967</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>1036257394</t>
+          <t>1055859437</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>111101110001000000100001110010</t>
+          <t>111110111011110010001011101101</t>
         </is>
       </c>
     </row>
@@ -1486,22 +1486,22 @@
         <v>43</v>
       </c>
       <c r="B44" t="n">
-        <v>0.9313985248163243</v>
+        <v>0.9669690522528936</v>
       </c>
       <c r="C44" t="n">
-        <v>0.7743047659351761</v>
+        <v>0.9669684954391649</v>
       </c>
       <c r="D44" t="n">
-        <v>0.7922</v>
+        <v>0.967</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>1036257394</t>
+          <t>1055859561</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>111101110001000000100001110010</t>
+          <t>111110111011110010001101101001</t>
         </is>
       </c>
     </row>
@@ -1510,22 +1510,22 @@
         <v>44</v>
       </c>
       <c r="B45" t="n">
-        <v>0.9313985248163243</v>
+        <v>0.9669690522528936</v>
       </c>
       <c r="C45" t="n">
-        <v>0.7743047659351761</v>
+        <v>0.9669685027656603</v>
       </c>
       <c r="D45" t="n">
-        <v>0.8035</v>
+        <v>0.967</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>1036257394</t>
+          <t>1055859561</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>111101110001000000100001110010</t>
+          <t>111110111011110010001101101001</t>
         </is>
       </c>
     </row>
@@ -1534,22 +1534,22 @@
         <v>45</v>
       </c>
       <c r="B46" t="n">
-        <v>0.9313985248163243</v>
+        <v>0.9669690522528936</v>
       </c>
       <c r="C46" t="n">
-        <v>0.7688922337375197</v>
+        <v>0.9669685027656603</v>
       </c>
       <c r="D46" t="n">
-        <v>0.8102</v>
+        <v>0.967</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>1036257394</t>
+          <t>1055859561</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>111101110001000000100001110010</t>
+          <t>111110111011110010001101101001</t>
         </is>
       </c>
     </row>
@@ -1558,22 +1558,22 @@
         <v>46</v>
       </c>
       <c r="B47" t="n">
-        <v>0.9313985248163243</v>
+        <v>0.9669690522528936</v>
       </c>
       <c r="C47" t="n">
-        <v>0.7743047659351761</v>
+        <v>0.8714985723076736</v>
       </c>
       <c r="D47" t="n">
-        <v>0.8196</v>
+        <v>0.9574</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>1036257394</t>
+          <t>1055859561</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>111101110001000000100001110010</t>
+          <t>111110111011110010001101101001</t>
         </is>
       </c>
     </row>
@@ -1582,22 +1582,22 @@
         <v>47</v>
       </c>
       <c r="B48" t="n">
-        <v>0.9313985248163243</v>
+        <v>0.966968825131485</v>
       </c>
       <c r="C48" t="n">
-        <v>0.8020472155884969</v>
+        <v>0.9669684954391649</v>
       </c>
       <c r="D48" t="n">
-        <v>0.8234</v>
+        <v>0.967</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>1036257394</t>
+          <t>1055859437</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>111101110001000000100001110010</t>
+          <t>111110111011110010001011101101</t>
         </is>
       </c>
     </row>
@@ -1606,22 +1606,22 @@
         <v>48</v>
       </c>
       <c r="B49" t="n">
-        <v>0.9313985248163243</v>
+        <v>0.9669688178049883</v>
       </c>
       <c r="C49" t="n">
-        <v>0.8020472155884969</v>
+        <v>0.9669684954391649</v>
       </c>
       <c r="D49" t="n">
-        <v>0.8234</v>
+        <v>0.967</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>1036257394</t>
+          <t>1055859433</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>111101110001000000100001110010</t>
+          <t>111110111011110010001011101001</t>
         </is>
       </c>
     </row>
@@ -1630,22 +1630,22 @@
         <v>49</v>
       </c>
       <c r="B50" t="n">
-        <v>0.9313985248163243</v>
+        <v>0.9669688178049883</v>
       </c>
       <c r="C50" t="n">
-        <v>0.8020472155884969</v>
+        <v>0.9669684954391649</v>
       </c>
       <c r="D50" t="n">
-        <v>0.8234</v>
+        <v>0.967</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>1036257394</t>
+          <t>1055859433</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>111101110001000000100001110010</t>
+          <t>111110111011110010001011101001</t>
         </is>
       </c>
     </row>
@@ -1654,22 +1654,22 @@
         <v>50</v>
       </c>
       <c r="B51" t="n">
-        <v>0.9313985248163243</v>
+        <v>0.9669688178049883</v>
       </c>
       <c r="C51" t="n">
-        <v>0.8020472155884969</v>
+        <v>0.9669685027656603</v>
       </c>
       <c r="D51" t="n">
-        <v>0.8234</v>
+        <v>0.967</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>1036257394</t>
+          <t>1055859433</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>111101110001000000100001110010</t>
+          <t>111110111011110010001011101001</t>
         </is>
       </c>
     </row>
@@ -1678,22 +1678,22 @@
         <v>51</v>
       </c>
       <c r="B52" t="n">
-        <v>0.9313985248163243</v>
+        <v>0.9669688178049883</v>
       </c>
       <c r="C52" t="n">
-        <v>0.8020472155884969</v>
+        <v>0.9669685027656603</v>
       </c>
       <c r="D52" t="n">
-        <v>0.8234</v>
+        <v>0.967</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>1036257394</t>
+          <t>1055859433</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>111101110001000000100001110010</t>
+          <t>111110111011110010001011101001</t>
         </is>
       </c>
     </row>
@@ -1702,22 +1702,22 @@
         <v>52</v>
       </c>
       <c r="B53" t="n">
-        <v>0.9313985248163243</v>
+        <v>0.9669688178049883</v>
       </c>
       <c r="C53" t="n">
-        <v>0.8020472155884969</v>
+        <v>0.9669685027656603</v>
       </c>
       <c r="D53" t="n">
-        <v>0.8234</v>
+        <v>0.967</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>1036257394</t>
+          <t>1055859433</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>111101110001000000100001110010</t>
+          <t>111110111011110010001011101001</t>
         </is>
       </c>
     </row>
@@ -1726,22 +1726,22 @@
         <v>53</v>
       </c>
       <c r="B54" t="n">
-        <v>0.9313985248163243</v>
+        <v>0.9686500704452468</v>
       </c>
       <c r="C54" t="n">
-        <v>0.7950122684638372</v>
+        <v>0.9669685027656603</v>
       </c>
       <c r="D54" t="n">
-        <v>0.8227</v>
+        <v>0.9671</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>1036257394</t>
+          <t>1056776937</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>111101110001000000100001110010</t>
+          <t>111110111111010010001011101001</t>
         </is>
       </c>
     </row>
@@ -1750,22 +1750,22 @@
         <v>54</v>
       </c>
       <c r="B55" t="n">
-        <v>0.9313985248163243</v>
+        <v>0.9686500704452468</v>
       </c>
       <c r="C55" t="n">
-        <v>0.8007358939451156</v>
+        <v>0.9669685027656603</v>
       </c>
       <c r="D55" t="n">
-        <v>0.8233</v>
+        <v>0.9676</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>1036257394</t>
+          <t>1056776937</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>111101110001000000100001110010</t>
+          <t>111110111111010010001011101001</t>
         </is>
       </c>
     </row>
@@ -1774,22 +1774,22 @@
         <v>55</v>
       </c>
       <c r="B56" t="n">
-        <v>0.9313985248163243</v>
+        <v>0.9686500704452468</v>
       </c>
       <c r="C56" t="n">
-        <v>0.8020446533416774</v>
+        <v>0.9669688178049883</v>
       </c>
       <c r="D56" t="n">
-        <v>0.8234</v>
+        <v>0.9685</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>1036257394</t>
+          <t>1056776937</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>111101110001000000100001110010</t>
+          <t>111110111111010010001011101001</t>
         </is>
       </c>
     </row>
@@ -1798,22 +1798,22 @@
         <v>56</v>
       </c>
       <c r="B57" t="n">
-        <v>0.9313985248163243</v>
+        <v>0.9686500704452468</v>
       </c>
       <c r="C57" t="n">
-        <v>0.8020446533416774</v>
+        <v>0.7457549446982441</v>
       </c>
       <c r="D57" t="n">
-        <v>0.8234</v>
+        <v>0.9464</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>1036257394</t>
+          <t>1056776937</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>111101110001000000100001110010</t>
+          <t>111110111111010010001011101001</t>
         </is>
       </c>
     </row>
@@ -1822,22 +1822,22 @@
         <v>57</v>
       </c>
       <c r="B58" t="n">
-        <v>0.9313985248163243</v>
+        <v>0.9686500704452468</v>
       </c>
       <c r="C58" t="n">
-        <v>0.8020465800307987</v>
+        <v>0.9686497551321607</v>
       </c>
       <c r="D58" t="n">
-        <v>0.8234</v>
+        <v>0.9686</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>1036257394</t>
+          <t>1056776937</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>111101110001000000100001110010</t>
+          <t>111110111111010010001011101001</t>
         </is>
       </c>
     </row>
@@ -1846,22 +1846,22 @@
         <v>58</v>
       </c>
       <c r="B59" t="n">
-        <v>0.9313985248163243</v>
+        <v>0.9686500704452468</v>
       </c>
       <c r="C59" t="n">
-        <v>0.8020472155884969</v>
+        <v>0.9686497551321607</v>
       </c>
       <c r="D59" t="n">
-        <v>0.8234</v>
+        <v>0.9686</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>1036257394</t>
+          <t>1056776937</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>111101110001000000100001110010</t>
+          <t>111110111111010010001011101001</t>
         </is>
       </c>
     </row>
@@ -1870,22 +1870,22 @@
         <v>59</v>
       </c>
       <c r="B60" t="n">
-        <v>0.9313985248163243</v>
+        <v>0.9686500704452468</v>
       </c>
       <c r="C60" t="n">
-        <v>0.006880506244592829</v>
+        <v>0.9686497551321607</v>
       </c>
       <c r="D60" t="n">
-        <v>0.7439</v>
+        <v>0.9686</v>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>1036257394</t>
+          <t>1056776937</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>111101110001000000100001110010</t>
+          <t>111110111111010010001011101001</t>
         </is>
       </c>
     </row>
@@ -1894,22 +1894,22 @@
         <v>60</v>
       </c>
       <c r="B61" t="n">
-        <v>0.9313985248163243</v>
+        <v>0.9686500704452468</v>
       </c>
       <c r="C61" t="n">
-        <v>0.8020472155884969</v>
+        <v>0.9686497551321607</v>
       </c>
       <c r="D61" t="n">
-        <v>0.8234</v>
+        <v>0.9686</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>1036257394</t>
+          <t>1056776937</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>111101110001000000100001110010</t>
+          <t>111110111111010010001011101001</t>
         </is>
       </c>
     </row>
@@ -1918,22 +1918,22 @@
         <v>61</v>
       </c>
       <c r="B62" t="n">
-        <v>0.9313985248163243</v>
+        <v>0.9686500704452468</v>
       </c>
       <c r="C62" t="n">
-        <v>0.8020472155884969</v>
+        <v>0.9686497551321607</v>
       </c>
       <c r="D62" t="n">
-        <v>0.8234</v>
+        <v>0.9686</v>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>1036257394</t>
+          <t>1056776937</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>111101110001000000100001110010</t>
+          <t>111110111111010010001011101001</t>
         </is>
       </c>
     </row>
@@ -1942,22 +1942,22 @@
         <v>62</v>
       </c>
       <c r="B63" t="n">
-        <v>0.9313985248163243</v>
+        <v>0.9686500704452468</v>
       </c>
       <c r="C63" t="n">
-        <v>0.8020472155884969</v>
+        <v>0.9686497551321607</v>
       </c>
       <c r="D63" t="n">
-        <v>0.8234</v>
+        <v>0.9686</v>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>1036257394</t>
+          <t>1056776937</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>111101110001000000100001110010</t>
+          <t>111110111111010010001011101001</t>
         </is>
       </c>
     </row>
@@ -1966,22 +1966,22 @@
         <v>63</v>
       </c>
       <c r="B64" t="n">
-        <v>0.9313985248163243</v>
+        <v>0.9686500704452468</v>
       </c>
       <c r="C64" t="n">
-        <v>0.8020472155884969</v>
+        <v>0.9686497551321607</v>
       </c>
       <c r="D64" t="n">
-        <v>0.8234</v>
+        <v>0.9686</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>1036257394</t>
+          <t>1056776937</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>111101110001000000100001110010</t>
+          <t>111110111111010010001011101001</t>
         </is>
       </c>
     </row>
@@ -1990,22 +1990,22 @@
         <v>64</v>
       </c>
       <c r="B65" t="n">
-        <v>0.9313985248163243</v>
+        <v>0.9686500777781099</v>
       </c>
       <c r="C65" t="n">
-        <v>0.8020472155884969</v>
+        <v>0.9686497477992989</v>
       </c>
       <c r="D65" t="n">
-        <v>0.8235</v>
+        <v>0.9686</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>1036257394</t>
+          <t>1056776941</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>111101110001000000100001110010</t>
+          <t>111110111111010010001011101101</t>
         </is>
       </c>
     </row>
@@ -2014,22 +2014,22 @@
         <v>65</v>
       </c>
       <c r="B66" t="n">
-        <v>0.9313985248163243</v>
+        <v>0.9686500704452468</v>
       </c>
       <c r="C66" t="n">
-        <v>0.8020472155884969</v>
+        <v>0.9686497477992989</v>
       </c>
       <c r="D66" t="n">
-        <v>0.8235</v>
+        <v>0.9686</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>1036257394</t>
+          <t>1056776937</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>111101110001000000100001110010</t>
+          <t>111110111111010010001011101001</t>
         </is>
       </c>
     </row>
@@ -2038,22 +2038,22 @@
         <v>66</v>
       </c>
       <c r="B67" t="n">
-        <v>0.9313985248163243</v>
+        <v>0.9686500704452468</v>
       </c>
       <c r="C67" t="n">
-        <v>0.8020472155884969</v>
+        <v>0.9686497477992989</v>
       </c>
       <c r="D67" t="n">
-        <v>0.8235</v>
+        <v>0.9686</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>1036257394</t>
+          <t>1056776937</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>111101110001000000100001110010</t>
+          <t>111110111111010010001011101001</t>
         </is>
       </c>
     </row>
@@ -2062,22 +2062,22 @@
         <v>67</v>
       </c>
       <c r="B68" t="n">
-        <v>0.9313985248163243</v>
+        <v>0.9686500777781099</v>
       </c>
       <c r="C68" t="n">
-        <v>0.8020472155884969</v>
+        <v>0.9686497477992989</v>
       </c>
       <c r="D68" t="n">
-        <v>0.8235</v>
+        <v>0.9686</v>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>1036257394</t>
+          <t>1056776941</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>111101110001000000100001110010</t>
+          <t>111110111111010010001011101101</t>
         </is>
       </c>
     </row>
@@ -2086,22 +2086,22 @@
         <v>68</v>
       </c>
       <c r="B69" t="n">
-        <v>0.9313985248163243</v>
+        <v>0.9686500777781099</v>
       </c>
       <c r="C69" t="n">
-        <v>0.8020472155884969</v>
+        <v>0.9686497477992989</v>
       </c>
       <c r="D69" t="n">
-        <v>0.8235</v>
+        <v>0.9686</v>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>1036257394</t>
+          <t>1056776941</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>111101110001000000100001110010</t>
+          <t>111110111111010010001011101101</t>
         </is>
       </c>
     </row>
@@ -2110,22 +2110,22 @@
         <v>69</v>
       </c>
       <c r="B70" t="n">
-        <v>0.9313985248163243</v>
+        <v>0.9686500704452468</v>
       </c>
       <c r="C70" t="n">
-        <v>0.8020472155884969</v>
+        <v>0.9686497477992989</v>
       </c>
       <c r="D70" t="n">
-        <v>0.8235</v>
+        <v>0.9686</v>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>1036257394</t>
+          <t>1056776937</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>111101110001000000100001110010</t>
+          <t>111110111111010010001011101001</t>
         </is>
       </c>
     </row>
@@ -2134,22 +2134,22 @@
         <v>70</v>
       </c>
       <c r="B71" t="n">
-        <v>0.9313985248163243</v>
+        <v>0.9957483956729301</v>
       </c>
       <c r="C71" t="n">
-        <v>0.8020918320345918</v>
+        <v>0.9686497477992989</v>
       </c>
       <c r="D71" t="n">
-        <v>0.8235</v>
+        <v>0.9714</v>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>1036257394</t>
+          <t>1071456829</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t>111101110001000000100001110010</t>
+          <t>111111110111010010001000111101</t>
         </is>
       </c>
     </row>
@@ -2158,22 +2158,22 @@
         <v>71</v>
       </c>
       <c r="B72" t="n">
-        <v>0.9313985248163243</v>
+        <v>0.9957483956729301</v>
       </c>
       <c r="C72" t="n">
-        <v>0.8020918320345918</v>
+        <v>0.9686497551321607</v>
       </c>
       <c r="D72" t="n">
-        <v>0.8235</v>
+        <v>0.9714</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>1036257394</t>
+          <t>1071456829</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>111101110001000000100001110010</t>
+          <t>111111110111010010001000111101</t>
         </is>
       </c>
     </row>
@@ -2182,22 +2182,22 @@
         <v>72</v>
       </c>
       <c r="B73" t="n">
-        <v>0.9313985248163243</v>
+        <v>0.9957483956729301</v>
       </c>
       <c r="C73" t="n">
-        <v>0.3213189432287343</v>
+        <v>0.9686497551321607</v>
       </c>
       <c r="D73" t="n">
-        <v>0.7272999999999999</v>
+        <v>0.9714</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>1036257394</t>
+          <t>1071456829</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>111101110001000000100001110010</t>
+          <t>111111110111010010001000111101</t>
         </is>
       </c>
     </row>
@@ -2206,22 +2206,22 @@
         <v>73</v>
       </c>
       <c r="B74" t="n">
-        <v>0.9313985248163243</v>
+        <v>0.9957483956729301</v>
       </c>
       <c r="C74" t="n">
-        <v>0.8020918320345918</v>
+        <v>0.9686497551321607</v>
       </c>
       <c r="D74" t="n">
-        <v>0.8235</v>
+        <v>0.9714</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>1036257394</t>
+          <t>1071456829</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>111101110001000000100001110010</t>
+          <t>111111110111010010001000111101</t>
         </is>
       </c>
     </row>
@@ -2230,22 +2230,22 @@
         <v>74</v>
       </c>
       <c r="B75" t="n">
-        <v>0.9313985248163243</v>
+        <v>0.9957483956729301</v>
       </c>
       <c r="C75" t="n">
-        <v>0.8020918320345918</v>
+        <v>0.9686497551321607</v>
       </c>
       <c r="D75" t="n">
-        <v>0.8235</v>
+        <v>0.9714</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>1036257394</t>
+          <t>1071456829</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>111101110001000000100001110010</t>
+          <t>111111110111010010001000111101</t>
         </is>
       </c>
     </row>
@@ -2254,22 +2254,22 @@
         <v>75</v>
       </c>
       <c r="B76" t="n">
-        <v>0.9313985248163243</v>
+        <v>0.9957483956729301</v>
       </c>
       <c r="C76" t="n">
-        <v>0.8020918320345918</v>
+        <v>0.9686497551321607</v>
       </c>
       <c r="D76" t="n">
-        <v>0.8235</v>
+        <v>0.9714</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>1036257394</t>
+          <t>1071456829</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>111101110001000000100001110010</t>
+          <t>111111110111010010001000111101</t>
         </is>
       </c>
     </row>
@@ -2278,22 +2278,22 @@
         <v>76</v>
       </c>
       <c r="B77" t="n">
-        <v>0.9313985248163243</v>
+        <v>0.9957483956729301</v>
       </c>
       <c r="C77" t="n">
-        <v>0.8020918320345918</v>
+        <v>0.968199276486002</v>
       </c>
       <c r="D77" t="n">
-        <v>0.8235</v>
+        <v>0.9713000000000001</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>1036257394</t>
+          <t>1071456829</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>111101110001000000100001110010</t>
+          <t>111111110111010010001000111101</t>
         </is>
       </c>
     </row>
@@ -2302,22 +2302,22 @@
         <v>77</v>
       </c>
       <c r="B78" t="n">
-        <v>0.9313985248163243</v>
+        <v>0.9957483956729301</v>
       </c>
       <c r="C78" t="n">
-        <v>0.8020918320345918</v>
+        <v>0.9686497551321607</v>
       </c>
       <c r="D78" t="n">
-        <v>0.8235</v>
+        <v>0.9714</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>1036257394</t>
+          <t>1071456829</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>111101110001000000100001110010</t>
+          <t>111111110111010010001000111101</t>
         </is>
       </c>
     </row>
@@ -2326,22 +2326,22 @@
         <v>78</v>
       </c>
       <c r="B79" t="n">
-        <v>0.9313985248163243</v>
+        <v>0.9957483956729301</v>
       </c>
       <c r="C79" t="n">
-        <v>0.8020918320345918</v>
+        <v>0.9686497551321607</v>
       </c>
       <c r="D79" t="n">
-        <v>0.8235</v>
+        <v>0.9714</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>1036257394</t>
+          <t>1071456829</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>111101110001000000100001110010</t>
+          <t>111111110111010010001000111101</t>
         </is>
       </c>
     </row>
@@ -2350,22 +2350,22 @@
         <v>79</v>
       </c>
       <c r="B80" t="n">
-        <v>0.9313985248163243</v>
+        <v>0.9957483956729301</v>
       </c>
       <c r="C80" t="n">
-        <v>0.8020918320345918</v>
+        <v>0.9686497551321607</v>
       </c>
       <c r="D80" t="n">
-        <v>0.8235</v>
+        <v>0.9714</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>1036257394</t>
+          <t>1071456829</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>111101110001000000100001110010</t>
+          <t>111111110111010010001000111101</t>
         </is>
       </c>
     </row>
@@ -2374,22 +2374,22 @@
         <v>80</v>
       </c>
       <c r="B81" t="n">
-        <v>0.9313985248163243</v>
+        <v>0.9957483956729301</v>
       </c>
       <c r="C81" t="n">
-        <v>0.8020918320345918</v>
+        <v>0.9686497551321607</v>
       </c>
       <c r="D81" t="n">
-        <v>0.8235</v>
+        <v>0.9714</v>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>1036257394</t>
+          <t>1071456829</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>111101110001000000100001110010</t>
+          <t>111111110111010010001000111101</t>
         </is>
       </c>
     </row>
@@ -2398,22 +2398,22 @@
         <v>81</v>
       </c>
       <c r="B82" t="n">
-        <v>0.9313985248163243</v>
+        <v>0.9957483956729301</v>
       </c>
       <c r="C82" t="n">
-        <v>0.8020918320345918</v>
+        <v>0.9684094868156933</v>
       </c>
       <c r="D82" t="n">
-        <v>0.8235</v>
+        <v>0.9713000000000001</v>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>1036257394</t>
+          <t>1071456829</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>111101110001000000100001110010</t>
+          <t>111111110111010010001000111101</t>
         </is>
       </c>
     </row>
@@ -2422,22 +2422,22 @@
         <v>82</v>
       </c>
       <c r="B83" t="n">
-        <v>0.9313985248163243</v>
+        <v>0.9957483956729301</v>
       </c>
       <c r="C83" t="n">
-        <v>0.8020918320345918</v>
+        <v>0.9686497551321607</v>
       </c>
       <c r="D83" t="n">
-        <v>0.8235</v>
+        <v>0.9714</v>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>1036257394</t>
+          <t>1071456829</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>111101110001000000100001110010</t>
+          <t>111111110111010010001000111101</t>
         </is>
       </c>
     </row>
@@ -2446,22 +2446,22 @@
         <v>83</v>
       </c>
       <c r="B84" t="n">
-        <v>0.9313985248163243</v>
+        <v>0.9957483956729301</v>
       </c>
       <c r="C84" t="n">
-        <v>0.8020918320345918</v>
+        <v>0.8963775158193851</v>
       </c>
       <c r="D84" t="n">
-        <v>0.8235</v>
+        <v>0.9569</v>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>1036257394</t>
+          <t>1071456829</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>111101110001000000100001110010</t>
+          <t>111111110111010010001000111101</t>
         </is>
       </c>
     </row>
@@ -2470,22 +2470,22 @@
         <v>84</v>
       </c>
       <c r="B85" t="n">
-        <v>0.9313985248163243</v>
+        <v>0.9957483956729301</v>
       </c>
       <c r="C85" t="n">
-        <v>0.8020918320345918</v>
+        <v>0.8960561078606716</v>
       </c>
       <c r="D85" t="n">
-        <v>0.8235</v>
+        <v>0.9641</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>1036257394</t>
+          <t>1071456829</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>111101110001000000100001110010</t>
+          <t>111111110111010010001000111101</t>
         </is>
       </c>
     </row>
@@ -2494,22 +2494,22 @@
         <v>85</v>
       </c>
       <c r="B86" t="n">
-        <v>0.9313985248163243</v>
+        <v>0.9957483956729301</v>
       </c>
       <c r="C86" t="n">
-        <v>0.8020918320345918</v>
+        <v>0.9686497532989452</v>
       </c>
       <c r="D86" t="n">
-        <v>0.8235</v>
+        <v>0.9714</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>1036257394</t>
+          <t>1071456829</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
         <is>
-          <t>111101110001000000100001110010</t>
+          <t>111111110111010010001000111101</t>
         </is>
       </c>
     </row>
@@ -2518,22 +2518,22 @@
         <v>86</v>
       </c>
       <c r="B87" t="n">
-        <v>0.9313985248163243</v>
+        <v>0.9957483956729301</v>
       </c>
       <c r="C87" t="n">
-        <v>0.8020918320345918</v>
+        <v>0.9686497532989452</v>
       </c>
       <c r="D87" t="n">
-        <v>0.8235</v>
+        <v>0.9714</v>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>1036257394</t>
+          <t>1071456829</t>
         </is>
       </c>
       <c r="F87" t="inlineStr">
         <is>
-          <t>111101110001000000100001110010</t>
+          <t>111111110111010010001000111101</t>
         </is>
       </c>
     </row>
@@ -2542,22 +2542,22 @@
         <v>87</v>
       </c>
       <c r="B88" t="n">
-        <v>0.9313985248163243</v>
+        <v>0.9957483956729301</v>
       </c>
       <c r="C88" t="n">
-        <v>0.8020918320345918</v>
+        <v>0.9686497459660834</v>
       </c>
       <c r="D88" t="n">
-        <v>0.8235</v>
+        <v>0.9714</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>1036257394</t>
+          <t>1071456829</t>
         </is>
       </c>
       <c r="F88" t="inlineStr">
         <is>
-          <t>111101110001000000100001110010</t>
+          <t>111111110111010010001000111101</t>
         </is>
       </c>
     </row>
@@ -2566,22 +2566,22 @@
         <v>88</v>
       </c>
       <c r="B89" t="n">
-        <v>0.9313985248163243</v>
+        <v>0.9957483956729301</v>
       </c>
       <c r="C89" t="n">
-        <v>0.8020918320345918</v>
+        <v>0.9686497258007135</v>
       </c>
       <c r="D89" t="n">
-        <v>0.8235</v>
+        <v>0.9714</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>1036257394</t>
+          <t>1071456829</t>
         </is>
       </c>
       <c r="F89" t="inlineStr">
         <is>
-          <t>111101110001000000100001110010</t>
+          <t>111111110111010010001000111101</t>
         </is>
       </c>
     </row>
@@ -2590,22 +2590,22 @@
         <v>89</v>
       </c>
       <c r="B90" t="n">
-        <v>0.9313985248163243</v>
+        <v>0.9957483956729301</v>
       </c>
       <c r="C90" t="n">
-        <v>0.8020918320345918</v>
+        <v>0.9686497258007135</v>
       </c>
       <c r="D90" t="n">
-        <v>0.8235</v>
+        <v>0.9714</v>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>1036257394</t>
+          <t>1071456829</t>
         </is>
       </c>
       <c r="F90" t="inlineStr">
         <is>
-          <t>111101110001000000100001110010</t>
+          <t>111111110111010010001000111101</t>
         </is>
       </c>
     </row>
@@ -2614,22 +2614,22 @@
         <v>90</v>
       </c>
       <c r="B91" t="n">
-        <v>0.9313985248163243</v>
+        <v>0.9957483956729301</v>
       </c>
       <c r="C91" t="n">
-        <v>0.8020918320345918</v>
+        <v>0.9686497551321607</v>
       </c>
       <c r="D91" t="n">
-        <v>0.8235</v>
+        <v>0.9714</v>
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>1036257394</t>
+          <t>1071456829</t>
         </is>
       </c>
       <c r="F91" t="inlineStr">
         <is>
-          <t>111101110001000000100001110010</t>
+          <t>111111110111010010001000111101</t>
         </is>
       </c>
     </row>
@@ -2638,22 +2638,22 @@
         <v>91</v>
       </c>
       <c r="B92" t="n">
-        <v>0.9313985248163243</v>
+        <v>0.9957483956729301</v>
       </c>
       <c r="C92" t="n">
-        <v>0.8020914183267073</v>
+        <v>0.9686497551321607</v>
       </c>
       <c r="D92" t="n">
-        <v>0.8235</v>
+        <v>0.9714</v>
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>1036257394</t>
+          <t>1071456829</t>
         </is>
       </c>
       <c r="F92" t="inlineStr">
         <is>
-          <t>111101110001000000100001110010</t>
+          <t>111111110111010010001000111101</t>
         </is>
       </c>
     </row>
@@ -2662,22 +2662,22 @@
         <v>92</v>
       </c>
       <c r="B93" t="n">
-        <v>0.9313985248163243</v>
+        <v>0.9957483956729301</v>
       </c>
       <c r="C93" t="n">
-        <v>0.8020914183267073</v>
+        <v>0.9686497551321607</v>
       </c>
       <c r="D93" t="n">
-        <v>0.8235</v>
+        <v>0.9714</v>
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>1036257394</t>
+          <t>1071456829</t>
         </is>
       </c>
       <c r="F93" t="inlineStr">
         <is>
-          <t>111101110001000000100001110010</t>
+          <t>111111110111010010001000111101</t>
         </is>
       </c>
     </row>
@@ -2686,22 +2686,22 @@
         <v>93</v>
       </c>
       <c r="B94" t="n">
-        <v>0.9313985248163243</v>
+        <v>0.9957483956729301</v>
       </c>
       <c r="C94" t="n">
-        <v>0.8020914183267073</v>
+        <v>0.9686497551321607</v>
       </c>
       <c r="D94" t="n">
-        <v>0.8235</v>
+        <v>0.9714</v>
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>1036257394</t>
+          <t>1071456829</t>
         </is>
       </c>
       <c r="F94" t="inlineStr">
         <is>
-          <t>111101110001000000100001110010</t>
+          <t>111111110111010010001000111101</t>
         </is>
       </c>
     </row>
@@ -2710,22 +2710,22 @@
         <v>94</v>
       </c>
       <c r="B95" t="n">
-        <v>0.9313985248163243</v>
+        <v>0.9957483956729301</v>
       </c>
       <c r="C95" t="n">
-        <v>0.8020914183267073</v>
+        <v>0.9686497551321607</v>
       </c>
       <c r="D95" t="n">
-        <v>0.8235</v>
+        <v>0.9714</v>
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>1036257394</t>
+          <t>1071456829</t>
         </is>
       </c>
       <c r="F95" t="inlineStr">
         <is>
-          <t>111101110001000000100001110010</t>
+          <t>111111110111010010001000111101</t>
         </is>
       </c>
     </row>
@@ -2734,22 +2734,22 @@
         <v>95</v>
       </c>
       <c r="B96" t="n">
-        <v>0.9313985248163243</v>
+        <v>0.9957483956729301</v>
       </c>
       <c r="C96" t="n">
-        <v>0.8020914183267073</v>
+        <v>0.9686497551321607</v>
       </c>
       <c r="D96" t="n">
-        <v>0.8235</v>
+        <v>0.9714</v>
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>1036257394</t>
+          <t>1071456829</t>
         </is>
       </c>
       <c r="F96" t="inlineStr">
         <is>
-          <t>111101110001000000100001110010</t>
+          <t>111111110111010010001000111101</t>
         </is>
       </c>
     </row>
@@ -2758,22 +2758,22 @@
         <v>96</v>
       </c>
       <c r="B97" t="n">
-        <v>0.9313985248163243</v>
+        <v>0.9957483956729301</v>
       </c>
       <c r="C97" t="n">
-        <v>0.8020914183267073</v>
+        <v>0.9618333111440945</v>
       </c>
       <c r="D97" t="n">
-        <v>0.8235</v>
+        <v>0.9707</v>
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>1036257394</t>
+          <t>1071456829</t>
         </is>
       </c>
       <c r="F97" t="inlineStr">
         <is>
-          <t>111101110001000000100001110010</t>
+          <t>111111110111010010001000111101</t>
         </is>
       </c>
     </row>
@@ -2782,22 +2782,22 @@
         <v>97</v>
       </c>
       <c r="B98" t="n">
-        <v>0.9313985248163243</v>
+        <v>0.9957483956729301</v>
       </c>
       <c r="C98" t="n">
-        <v>0.8020914183267073</v>
+        <v>0.9686497551321607</v>
       </c>
       <c r="D98" t="n">
-        <v>0.8235</v>
+        <v>0.9714</v>
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>1036257394</t>
+          <t>1071456829</t>
         </is>
       </c>
       <c r="F98" t="inlineStr">
         <is>
-          <t>111101110001000000100001110010</t>
+          <t>111111110111010010001000111101</t>
         </is>
       </c>
     </row>
@@ -2806,22 +2806,22 @@
         <v>98</v>
       </c>
       <c r="B99" t="n">
-        <v>0.9313985248163243</v>
+        <v>0.9957483956729301</v>
       </c>
       <c r="C99" t="n">
-        <v>0.8020913933040564</v>
+        <v>0.9686497294671443</v>
       </c>
       <c r="D99" t="n">
-        <v>0.8235</v>
+        <v>0.9714</v>
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>1036257394</t>
+          <t>1071456829</t>
         </is>
       </c>
       <c r="F99" t="inlineStr">
         <is>
-          <t>111101110001000000100001110010</t>
+          <t>111111110111010010001000111101</t>
         </is>
       </c>
     </row>
@@ -2830,22 +2830,22 @@
         <v>99</v>
       </c>
       <c r="B100" t="n">
-        <v>0.9313985248163243</v>
+        <v>0.9957483956729301</v>
       </c>
       <c r="C100" t="n">
-        <v>0.8020913933040564</v>
+        <v>0.8785898999344711</v>
       </c>
       <c r="D100" t="n">
-        <v>0.8235</v>
+        <v>0.9624</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>1036257394</t>
+          <t>1071456829</t>
         </is>
       </c>
       <c r="F100" t="inlineStr">
         <is>
-          <t>111101110001000000100001110010</t>
+          <t>111111110111010010001000111101</t>
         </is>
       </c>
     </row>
@@ -2854,22 +2854,22 @@
         <v>100</v>
       </c>
       <c r="B101" t="n">
-        <v>0.9313985248163243</v>
+        <v>0.9957483956729301</v>
       </c>
       <c r="C101" t="n">
-        <v>0.8020715354513778</v>
+        <v>0.9686497294671443</v>
       </c>
       <c r="D101" t="n">
-        <v>0.8249</v>
+        <v>0.9714</v>
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>1036257394</t>
+          <t>1071456829</t>
         </is>
       </c>
       <c r="F101" t="inlineStr">
         <is>
-          <t>111101110001000000100001110010</t>
+          <t>111111110111010010001000111101</t>
         </is>
       </c>
     </row>

</xml_diff>